<commit_message>
📅 Monthly schedule for 06/2025
</commit_message>
<xml_diff>
--- a/schedule_06_2025.xlsx
+++ b/schedule_06_2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
   <si>
     <t>June 2025</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Sun</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -56,6 +59,12 @@
     <t>6</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>9AM-11AM: a a, b b, c c</t>
   </si>
   <si>
@@ -122,6 +131,12 @@
     <t>13</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
@@ -137,6 +152,12 @@
     <t>20</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>23</t>
   </si>
   <si>
@@ -150,6 +171,12 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
   </si>
   <si>
     <t>30</t>
@@ -580,369 +607,398 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1">
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" customHeight="1">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" customHeight="1">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="21" spans="1:7" ht="30" customHeight="1">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="E16" t="s">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" t="s">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E21" t="s">
         <v>28</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="22" spans="1:7" ht="30" customHeight="1">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="s">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" customHeight="1">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" customHeight="1">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" customHeight="1">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" customHeight="1">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" customHeight="1">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" customHeight="1">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" customHeight="1">
+      <c r="A29" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="30" customHeight="1">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="31" spans="1:7" ht="30" customHeight="1">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="30" customHeight="1">
+      <c r="A32" t="s">
         <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" customHeight="1">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" customHeight="1">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" customHeight="1">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" customHeight="1">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" customHeight="1">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" customHeight="1">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1">
-      <c r="A32" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -963,57 +1019,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>